<commit_message>
Updating lease_import to match model changes
</commit_message>
<xml_diff>
--- a/app/private/lease_import_v2.xlsx
+++ b/app/private/lease_import_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr date1904="1" showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27820" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="27820" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="building_modele_import_building" sheetId="1" r:id="rId1"/>
@@ -1182,6 +1182,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="BU1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+new_dvr, good_dvr, average_dvr, bad_dvr</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="BV1" authorId="0">
       <text>
         <r>
@@ -1202,11 +1226,35 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BX1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 new_dvr, good_dvr, average_dvr, bad_dvr</t>
         </r>
       </text>
     </comment>
-    <comment ref="BW1" authorId="0">
+    <comment ref="BY1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1230,7 +1278,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BZ1" authorId="0">
+    <comment ref="CA1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1254,7 +1302,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CA1" authorId="0">
+    <comment ref="CB1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1326,6 +1374,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="CG1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+new_dvr, good_dvr, average_dvr, bad_dvr</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="CH1" authorId="0">
       <text>
         <r>
@@ -1346,11 +1418,35 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CJ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 new_dvr, good_dvr, average_dvr, bad_dvr</t>
         </r>
       </text>
     </comment>
-    <comment ref="CI1" authorId="0">
+    <comment ref="CK1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1374,7 +1470,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CL1" authorId="0">
+    <comment ref="CM1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1398,7 +1494,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CM1" authorId="0">
+    <comment ref="CN1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1422,31 +1518,103 @@
         </r>
       </text>
     </comment>
-    <comment ref="CP1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Benjamin-Samuel Ewenczyk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-new_dvr, good_dvr, average_dvr, bad_dvr</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CQ1" authorId="0">
+    <comment ref="DT1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Commentaires généraux</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DU1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+true, false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DV1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DW1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ex : 2014-12-20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DX1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1470,31 +1638,79 @@
         </r>
       </text>
     </comment>
-    <comment ref="CT1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Benjamin-Samuel Ewenczyk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-new_dvr, good_dvr, average_dvr, bad_dvr</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CU1" authorId="0">
+    <comment ref="DZ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+true, false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EA1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EB1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ex : 2014-12-20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EC1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1518,6 +1734,126 @@
         </r>
       </text>
     </comment>
+    <comment ref="EE1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+true, false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EF1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EG1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ex : 2014-12-20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EH1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EJ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+true, false</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="EK1" authorId="0">
       <text>
         <r>
@@ -1538,7 +1874,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Commentaires généraux</t>
+monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
         </r>
       </text>
     </comment>
@@ -1562,11 +1898,59 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
+Ex : 2014-12-20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EM1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EO1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 true, false</t>
         </r>
       </text>
     </comment>
-    <comment ref="EM1" authorId="0">
+    <comment ref="EP1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1590,7 +1974,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EN1" authorId="0">
+    <comment ref="EQ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1614,7 +1998,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EO1" authorId="0">
+    <comment ref="ER1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1638,7 +2022,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EQ1" authorId="0">
+    <comment ref="ET1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1662,7 +2046,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="ER1" authorId="0">
+    <comment ref="EU1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1686,7 +2070,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="ES1" authorId="0">
+    <comment ref="EV1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1710,7 +2094,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="ET1" authorId="0">
+    <comment ref="EW1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1734,7 +2118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EV1" authorId="0">
+    <comment ref="EY1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1758,7 +2142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EW1" authorId="0">
+    <comment ref="EZ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1782,7 +2166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EX1" authorId="0">
+    <comment ref="FA1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1806,7 +2190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EY1" authorId="0">
+    <comment ref="FB1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1830,7 +2214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FA1" authorId="0">
+    <comment ref="FD1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1854,7 +2238,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FB1" authorId="0">
+    <comment ref="FE1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1878,7 +2262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FC1" authorId="0">
+    <comment ref="FF1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1902,7 +2286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FD1" authorId="0">
+    <comment ref="FG1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1926,7 +2310,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FF1" authorId="0">
+    <comment ref="FI1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1950,7 +2334,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FG1" authorId="0">
+    <comment ref="FJ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1974,7 +2358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FH1" authorId="0">
+    <comment ref="FK1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1998,7 +2382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FI1" authorId="0">
+    <comment ref="FL1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2022,7 +2406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FK1" authorId="0">
+    <comment ref="FN1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2046,7 +2430,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FL1" authorId="0">
+    <comment ref="FO1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2070,7 +2454,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FM1" authorId="0">
+    <comment ref="FP1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2094,7 +2478,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FN1" authorId="0">
+    <comment ref="FQ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2118,7 +2502,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FP1" authorId="0">
+    <comment ref="FS1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2142,7 +2526,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FQ1" authorId="0">
+    <comment ref="FT1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2166,7 +2550,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FR1" authorId="0">
+    <comment ref="FU1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2190,7 +2574,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FS1" authorId="0">
+    <comment ref="FV1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2214,7 +2598,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FU1" authorId="0">
+    <comment ref="FX1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2238,7 +2622,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FV1" authorId="0">
+    <comment ref="FY1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2262,7 +2646,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FW1" authorId="0">
+    <comment ref="FZ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2286,7 +2670,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FX1" authorId="0">
+    <comment ref="GA1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2310,7 +2694,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FZ1" authorId="0">
+    <comment ref="GC1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2334,7 +2718,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="GA1" authorId="0">
+    <comment ref="GD1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2358,7 +2742,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="GB1" authorId="0">
+    <comment ref="GE1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2382,7 +2766,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="GC1" authorId="0">
+    <comment ref="GF1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2406,7 +2790,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="GE1" authorId="0">
+    <comment ref="GH1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2430,7 +2814,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="GF1" authorId="0">
+    <comment ref="GI1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2454,7 +2838,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="GG1" authorId="0">
+    <comment ref="GJ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2478,391 +2862,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="GH1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Benjamin-Samuel Ewenczyk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-compliant, not_compliant_minor, not_compliant_major</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="GJ1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Benjamin-Samuel Ewenczyk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-true, false</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="GK1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Benjamin-Samuel Ewenczyk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="GL1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Benjamin-Samuel Ewenczyk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Ex : 2014-12-20</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="GM1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Benjamin-Samuel Ewenczyk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-compliant, not_compliant_minor, not_compliant_major</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="GO1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Benjamin-Samuel Ewenczyk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-true, false</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="GP1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Benjamin-Samuel Ewenczyk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="GQ1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Benjamin-Samuel Ewenczyk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Ex : 2014-12-20</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="GR1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Benjamin-Samuel Ewenczyk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-compliant, not_compliant_minor, not_compliant_major</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="GT1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Benjamin-Samuel Ewenczyk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-true, false</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="GU1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Benjamin-Samuel Ewenczyk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="GV1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Benjamin-Samuel Ewenczyk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Ex : 2014-12-20</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="GW1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Benjamin-Samuel Ewenczyk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-compliant, not_compliant_minor, not_compliant_major</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="GY1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Benjamin-Samuel Ewenczyk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-true, false</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="GZ1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Benjamin-Samuel Ewenczyk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="HA1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Benjamin-Samuel Ewenczyk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Ex : 2014-12-20</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="HB1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2891,7 +2891,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="228">
   <si>
     <t>building_id</t>
   </si>
@@ -3187,264 +3187,9 @@
     <t>comfort_qualitative_assessment.comments</t>
   </si>
   <si>
-    <t>technical_compliance.0.name</t>
-  </si>
-  <si>
-    <t>technical_compliance.0.lifetime</t>
-  </si>
-  <si>
-    <t>technical_compliance.0.conformity</t>
-  </si>
-  <si>
-    <t>technical_compliance.0.description</t>
-  </si>
-  <si>
-    <t>Structure</t>
-  </si>
-  <si>
     <t>technical_compliance.tc_comments</t>
   </si>
   <si>
-    <t>technical_compliance.1.name</t>
-  </si>
-  <si>
-    <t>technical_compliance.1.lifetime</t>
-  </si>
-  <si>
-    <t>technical_compliance.1.conformity</t>
-  </si>
-  <si>
-    <t>technical_compliance.1.description</t>
-  </si>
-  <si>
-    <t>technical_compliance.2.name</t>
-  </si>
-  <si>
-    <t>technical_compliance.2.lifetime</t>
-  </si>
-  <si>
-    <t>technical_compliance.2.conformity</t>
-  </si>
-  <si>
-    <t>technical_compliance.2.description</t>
-  </si>
-  <si>
-    <t>technical_compliance.3.name</t>
-  </si>
-  <si>
-    <t>technical_compliance.3.lifetime</t>
-  </si>
-  <si>
-    <t>technical_compliance.3.conformity</t>
-  </si>
-  <si>
-    <t>technical_compliance.3.description</t>
-  </si>
-  <si>
-    <t>technical_compliance.4.name</t>
-  </si>
-  <si>
-    <t>technical_compliance.4.lifetime</t>
-  </si>
-  <si>
-    <t>technical_compliance.4.conformity</t>
-  </si>
-  <si>
-    <t>technical_compliance.4.description</t>
-  </si>
-  <si>
-    <t>technical_compliance.5.name</t>
-  </si>
-  <si>
-    <t>technical_compliance.5.lifetime</t>
-  </si>
-  <si>
-    <t>technical_compliance.5.conformity</t>
-  </si>
-  <si>
-    <t>technical_compliance.5.description</t>
-  </si>
-  <si>
-    <t>technical_compliance.6.name</t>
-  </si>
-  <si>
-    <t>technical_compliance.6.lifetime</t>
-  </si>
-  <si>
-    <t>technical_compliance.6.conformity</t>
-  </si>
-  <si>
-    <t>technical_compliance.6.description</t>
-  </si>
-  <si>
-    <t>technical_compliance.7.name</t>
-  </si>
-  <si>
-    <t>technical_compliance.7.lifetime</t>
-  </si>
-  <si>
-    <t>technical_compliance.7.conformity</t>
-  </si>
-  <si>
-    <t>technical_compliance.7.description</t>
-  </si>
-  <si>
-    <t>technical_compliance.8.name</t>
-  </si>
-  <si>
-    <t>technical_compliance.8.lifetime</t>
-  </si>
-  <si>
-    <t>technical_compliance.8.conformity</t>
-  </si>
-  <si>
-    <t>technical_compliance.8.description</t>
-  </si>
-  <si>
-    <t>technical_compliance.9.name</t>
-  </si>
-  <si>
-    <t>technical_compliance.9.lifetime</t>
-  </si>
-  <si>
-    <t>technical_compliance.9.conformity</t>
-  </si>
-  <si>
-    <t>technical_compliance.9.description</t>
-  </si>
-  <si>
-    <t>technical_compliance.10.name</t>
-  </si>
-  <si>
-    <t>technical_compliance.11.lifetime</t>
-  </si>
-  <si>
-    <t>technical_compliance.10.lifetime</t>
-  </si>
-  <si>
-    <t>technical_compliance.10.conformity</t>
-  </si>
-  <si>
-    <t>technical_compliance.10.description</t>
-  </si>
-  <si>
-    <t>technical_compliance.11.name</t>
-  </si>
-  <si>
-    <t>technical_compliance.11.conformity</t>
-  </si>
-  <si>
-    <t>technical_compliance.11.description</t>
-  </si>
-  <si>
-    <t>technical_compliance.12.name</t>
-  </si>
-  <si>
-    <t>technical_compliance.13.lifetime</t>
-  </si>
-  <si>
-    <t>technical_compliance.14.conformity</t>
-  </si>
-  <si>
-    <t>technical_compliance.12.lifetime</t>
-  </si>
-  <si>
-    <t>technical_compliance.12.conformity</t>
-  </si>
-  <si>
-    <t>technical_compliance.12.description</t>
-  </si>
-  <si>
-    <t>technical_compliance.13.name</t>
-  </si>
-  <si>
-    <t>technical_compliance.13.conformity</t>
-  </si>
-  <si>
-    <t>technical_compliance.13.description</t>
-  </si>
-  <si>
-    <t>technical_compliance.14.name</t>
-  </si>
-  <si>
-    <t>technical_compliance.14.lifetime</t>
-  </si>
-  <si>
-    <t>technical_compliance.14.description</t>
-  </si>
-  <si>
-    <t>technical_compliance.15.name</t>
-  </si>
-  <si>
-    <t>technical_compliance.15.lifetime</t>
-  </si>
-  <si>
-    <t>technical_compliance.15.conformity</t>
-  </si>
-  <si>
-    <t>technical_compliance.15.description</t>
-  </si>
-  <si>
-    <t>technical_compliance.16.name</t>
-  </si>
-  <si>
-    <t>technical_compliance.16.lifetime</t>
-  </si>
-  <si>
-    <t>technical_compliance.16.conformity</t>
-  </si>
-  <si>
-    <t>technical_compliance.16.description</t>
-  </si>
-  <si>
-    <t>Facade</t>
-  </si>
-  <si>
-    <t>Toiture / étanchéité</t>
-  </si>
-  <si>
-    <t>Production Chaud</t>
-  </si>
-  <si>
-    <t>Production Froid</t>
-  </si>
-  <si>
-    <t>TGBT</t>
-  </si>
-  <si>
-    <t>Distribution électrique</t>
-  </si>
-  <si>
-    <t>Distribution thermique</t>
-  </si>
-  <si>
-    <t>Terminaux chauffage</t>
-  </si>
-  <si>
-    <t>Terminaux climatisation</t>
-  </si>
-  <si>
-    <t>Terminaux d'éclairage</t>
-  </si>
-  <si>
-    <t>GTC/GTB</t>
-  </si>
-  <si>
-    <t>Centrales d'air</t>
-  </si>
-  <si>
-    <t>Réseaux ventilation</t>
-  </si>
-  <si>
-    <t>Production ECS</t>
-  </si>
-  <si>
-    <t>Distribution ECS</t>
-  </si>
-  <si>
-    <t>Sécurité incendie</t>
-  </si>
-  <si>
     <t>accessibility.eligibility</t>
   </si>
   <si>
@@ -3677,6 +3422,159 @@
   </si>
   <si>
     <t>bad</t>
+  </si>
+  <si>
+    <t>technical_compliance.core_and_shell.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.core_and_shell.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.core_and_shell.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.facade.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.facade.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.facade.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.roof_terrasse.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.roof_terrasse.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.roof_terrasse.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.heat_production.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.heat_production.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.heat_production.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.chiller.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.chiller.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.chiller.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.power_supply.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.power_supply.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.power_supply.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.electrical_delivery.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.electrical_delivery.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.electrical_delivery.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.thermal_delivery.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.thermal_delivery.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.thermal_delivery.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.heating_terminal.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.heating_terminal.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.heating_terminal.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.chiller_terminal.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.chiller_terminal.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.chiller_terminal.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.lighting_terminal.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.lighting_terminal.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.lighting_terminal.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.GTC_GTB.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.GTC_GTB.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.GTC_GTB.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.air_system.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.air_system.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.air_system.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.ventilation_system.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.ventilation_system.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.ventilation_system.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.hot_water_production.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.hot_water_production.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.hot_water_production.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.hot_water_delivery.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.hot_water_delivery.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.hot_water_delivery.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.fire_security.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.fire_security.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.fire_security.description</t>
   </si>
 </sst>
 </file>
@@ -4282,10 +4180,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:HC2"/>
+  <dimension ref="A1:GL2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BO1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="BT2" sqref="BT2"/>
+    <sheetView tabSelected="1" topLeftCell="DE1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="DS1" sqref="BU1:DS1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4360,79 +4258,12 @@
     <col min="70" max="70" width="19.33203125" customWidth="1"/>
     <col min="71" max="71" width="19.1640625" customWidth="1"/>
     <col min="72" max="72" width="19.5" customWidth="1"/>
-    <col min="73" max="73" width="18.6640625" customWidth="1"/>
-    <col min="74" max="74" width="18.5" customWidth="1"/>
-    <col min="75" max="75" width="18.83203125" customWidth="1"/>
-    <col min="76" max="76" width="18.5" customWidth="1"/>
-    <col min="77" max="77" width="18.6640625" customWidth="1"/>
-    <col min="78" max="78" width="18.5" customWidth="1"/>
-    <col min="79" max="79" width="18.83203125" customWidth="1"/>
-    <col min="80" max="80" width="18.5" customWidth="1"/>
-    <col min="81" max="81" width="18.6640625" customWidth="1"/>
-    <col min="82" max="82" width="18.5" customWidth="1"/>
-    <col min="83" max="83" width="18.83203125" customWidth="1"/>
-    <col min="84" max="84" width="18.5" customWidth="1"/>
-    <col min="85" max="85" width="18.6640625" customWidth="1"/>
-    <col min="86" max="86" width="18.5" customWidth="1"/>
-    <col min="87" max="87" width="18.83203125" customWidth="1"/>
-    <col min="88" max="88" width="18.5" customWidth="1"/>
-    <col min="89" max="89" width="18.6640625" customWidth="1"/>
-    <col min="90" max="90" width="18.5" customWidth="1"/>
-    <col min="91" max="91" width="18.83203125" customWidth="1"/>
-    <col min="92" max="92" width="18.5" customWidth="1"/>
-    <col min="93" max="93" width="18.6640625" customWidth="1"/>
-    <col min="94" max="94" width="18.5" customWidth="1"/>
-    <col min="95" max="95" width="18.83203125" customWidth="1"/>
-    <col min="96" max="96" width="18.5" customWidth="1"/>
-    <col min="97" max="97" width="18.6640625" customWidth="1"/>
-    <col min="98" max="98" width="18.5" customWidth="1"/>
-    <col min="99" max="99" width="18.83203125" customWidth="1"/>
-    <col min="100" max="100" width="18.5" customWidth="1"/>
-    <col min="101" max="101" width="18.6640625" customWidth="1"/>
-    <col min="102" max="102" width="18.5" customWidth="1"/>
-    <col min="103" max="103" width="18.83203125" customWidth="1"/>
-    <col min="104" max="104" width="18.5" customWidth="1"/>
-    <col min="105" max="105" width="18.6640625" customWidth="1"/>
-    <col min="106" max="106" width="18.5" customWidth="1"/>
-    <col min="107" max="107" width="18.83203125" customWidth="1"/>
-    <col min="108" max="108" width="18.5" customWidth="1"/>
-    <col min="109" max="109" width="18.6640625" customWidth="1"/>
-    <col min="110" max="110" width="18.5" customWidth="1"/>
-    <col min="111" max="111" width="18.83203125" customWidth="1"/>
-    <col min="112" max="112" width="18.5" customWidth="1"/>
-    <col min="113" max="113" width="18.6640625" customWidth="1"/>
-    <col min="114" max="114" width="18.5" customWidth="1"/>
-    <col min="115" max="115" width="18.83203125" customWidth="1"/>
-    <col min="116" max="116" width="18.5" customWidth="1"/>
-    <col min="117" max="117" width="18.6640625" customWidth="1"/>
-    <col min="118" max="118" width="18.5" customWidth="1"/>
-    <col min="119" max="119" width="18.83203125" customWidth="1"/>
-    <col min="120" max="120" width="18.5" customWidth="1"/>
-    <col min="121" max="121" width="18.6640625" customWidth="1"/>
-    <col min="122" max="122" width="18.5" customWidth="1"/>
-    <col min="123" max="123" width="18.83203125" customWidth="1"/>
-    <col min="124" max="124" width="18.5" customWidth="1"/>
-    <col min="125" max="125" width="18.6640625" customWidth="1"/>
-    <col min="126" max="126" width="18.5" customWidth="1"/>
-    <col min="127" max="127" width="18.83203125" customWidth="1"/>
-    <col min="128" max="128" width="18.5" customWidth="1"/>
-    <col min="129" max="129" width="18.6640625" customWidth="1"/>
-    <col min="130" max="130" width="18.5" customWidth="1"/>
-    <col min="131" max="131" width="18.83203125" customWidth="1"/>
-    <col min="132" max="132" width="18.5" customWidth="1"/>
-    <col min="133" max="133" width="18.6640625" customWidth="1"/>
-    <col min="134" max="134" width="18.5" customWidth="1"/>
-    <col min="135" max="135" width="18.83203125" customWidth="1"/>
-    <col min="136" max="136" width="18.5" customWidth="1"/>
-    <col min="137" max="137" width="18.6640625" customWidth="1"/>
-    <col min="138" max="138" width="18.5" customWidth="1"/>
-    <col min="139" max="139" width="18.83203125" customWidth="1"/>
-    <col min="140" max="140" width="18.5" customWidth="1"/>
-    <col min="141" max="141" width="16.6640625" customWidth="1"/>
-    <col min="142" max="211" width="20.5" customWidth="1"/>
+    <col min="73" max="123" width="26" customWidth="1"/>
+    <col min="124" max="124" width="31.33203125" customWidth="1"/>
+    <col min="125" max="194" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:211" s="1" customFormat="1" ht="30">
+    <row r="1" spans="1:194" s="1" customFormat="1" ht="45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4650,424 +4481,373 @@
         <v>97</v>
       </c>
       <c r="BU1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="BX1" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="BY1" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="BZ1" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="CD1" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="CE1" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="CF1" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="CI1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="CJ1" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="CK1" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="CL1" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="CM1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="CN1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="CO1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="CP1" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="CQ1" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="CR1" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="CS1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="CT1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="CU1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="CV1" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="CW1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="CX1" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="CY1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="CZ1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="DA1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="DB1" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="DC1" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="DD1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="DE1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="DF1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="DG1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="DH1" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="DI1" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DJ1" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="DK1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="DL1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="DM1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="DN1" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="DO1" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="DP1" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="DQ1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="DR1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="DS1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="DT1" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="DU1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="DV1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="DW1" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="BY1" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="BZ1" s="3" t="s">
+      <c r="DX1" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="CA1" s="3" t="s">
+      <c r="DY1" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="CB1" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="CC1" s="1" t="s">
+      <c r="DZ1" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="EA1" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="EB1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="EC1" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="CG1" s="3" t="s">
+      <c r="ED1" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="CH1" s="3" t="s">
+      <c r="EE1" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="CI1" s="3" t="s">
+      <c r="EF1" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="CJ1" s="3" t="s">
+      <c r="EG1" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="EH1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="CL1" s="1" t="s">
+      <c r="EI1" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="CM1" s="1" t="s">
+      <c r="EJ1" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="CN1" s="1" t="s">
+      <c r="EK1" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="CO1" s="3" t="s">
+      <c r="EL1" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="CP1" s="3" t="s">
+      <c r="EM1" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="CQ1" s="3" t="s">
+      <c r="EN1" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="CR1" s="3" t="s">
+      <c r="EO1" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="CS1" s="1" t="s">
+      <c r="EP1" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="CT1" s="1" t="s">
+      <c r="EQ1" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="CU1" s="1" t="s">
+      <c r="ER1" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="CV1" s="1" t="s">
+      <c r="ES1" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="CW1" s="3" t="s">
+      <c r="ET1" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="CX1" s="3" t="s">
+      <c r="EU1" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="CY1" s="3" t="s">
+      <c r="EV1" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="CZ1" s="3" t="s">
+      <c r="EW1" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="EX1" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="DB1" s="1" t="s">
+      <c r="EY1" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="DC1" s="1" t="s">
+      <c r="EZ1" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="DD1" s="1" t="s">
+      <c r="FA1" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="DE1" s="3" t="s">
+      <c r="FB1" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="DF1" s="3" t="s">
+      <c r="FC1" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="DG1" s="3" t="s">
+      <c r="FD1" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="DH1" s="3" t="s">
+      <c r="FE1" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="FF1" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="DJ1" s="1" t="s">
+      <c r="FG1" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="FH1" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="DK1" s="1" t="s">
+      <c r="FI1" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="DL1" s="1" t="s">
+      <c r="FJ1" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="DM1" s="3" t="s">
+      <c r="FK1" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="DN1" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="DO1" s="3" t="s">
+      <c r="FL1" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="DP1" s="3" t="s">
+      <c r="FM1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="DQ1" s="1" t="s">
+      <c r="FN1" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="DR1" s="1" t="s">
+      <c r="FO1" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="FP1" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="FQ1" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="DS1" s="1" t="s">
+      <c r="FR1" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="DT1" s="1" t="s">
+      <c r="FS1" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="DU1" s="3" t="s">
+      <c r="FT1" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="DV1" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="DW1" s="3" t="s">
+      <c r="FU1" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="DX1" s="3" t="s">
+      <c r="FV1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="DY1" s="1" t="s">
+      <c r="FW1" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="DZ1" s="1" t="s">
+      <c r="FX1" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="EA1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="EB1" s="1" t="s">
+      <c r="FY1" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="EC1" s="3" t="s">
+      <c r="FZ1" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="ED1" s="3" t="s">
+      <c r="GA1" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="EE1" s="3" t="s">
+      <c r="GB1" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="EF1" s="3" t="s">
+      <c r="GC1" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="EG1" s="1" t="s">
+      <c r="GD1" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="EH1" s="1" t="s">
+      <c r="GE1" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="EI1" s="1" t="s">
+      <c r="GF1" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="EJ1" s="1" t="s">
+      <c r="GG1" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="EK1" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="EL1" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="EM1" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="EN1" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="EO1" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="EP1" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="EQ1" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="ER1" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="ES1" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="ET1" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="EU1" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="EV1" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="EW1" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="EX1" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="EY1" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="EZ1" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="FA1" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="FB1" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="FC1" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="FD1" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="FE1" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="FF1" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="FG1" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="FH1" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="FI1" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="FJ1" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="FK1" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="FL1" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="FM1" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="FN1" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FO1" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="FP1" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="FQ1" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="FR1" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="FS1" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="FT1" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="FU1" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="FV1" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="FW1" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="FX1" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="FY1" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="FZ1" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="GA1" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="GB1" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="GC1" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="GD1" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="GE1" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="GF1" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="GG1" s="5" t="s">
-        <v>235</v>
-      </c>
       <c r="GH1" s="5" t="s">
-        <v>236</v>
+        <v>168</v>
       </c>
       <c r="GI1" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="GJ1" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="GK1" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="GL1" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="GM1" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="GN1" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="GO1" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="GP1" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="GQ1" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="GR1" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="GS1" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="GT1" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="GU1" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="GV1" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="GW1" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="GX1" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="GY1" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="GZ1" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="HA1" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="HB1" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="HC1" s="5" t="s">
-        <v>257</v>
+        <v>169</v>
+      </c>
+      <c r="GJ1" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="GK1" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="GL1" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:211" s="2" customFormat="1" ht="30">
+    <row r="2" spans="1:194" s="2" customFormat="1" ht="30">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -5234,334 +5014,283 @@
         <v>92</v>
       </c>
       <c r="BQ2" s="2" t="s">
-        <v>259</v>
+        <v>174</v>
       </c>
       <c r="BR2" s="2" t="s">
-        <v>260</v>
+        <v>175</v>
       </c>
       <c r="BS2" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="BU2" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="BU2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="BV2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="BX2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="BY2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="CA2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="CB2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="CD2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="CE2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="CG2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="CH2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="CJ2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="CK2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="CM2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="CN2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="CP2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="CQ2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="CS2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="CT2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="CV2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="CW2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="CY2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="CZ2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="DB2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="DC2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="DE2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="DF2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="DH2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="DI2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="DK2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="DL2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="DN2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="DO2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="DQ2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="DR2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="DU2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="DV2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="DW2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="BV2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="BW2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="BY2" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="BZ2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="CA2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="CC2" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="CD2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="CE2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="CG2" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="CH2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="CI2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="CK2" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="CL2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="CM2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="CO2" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="CP2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="CQ2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="CS2" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="CT2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="CU2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="CW2" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="CX2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="CY2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="DA2" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="DB2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="DC2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="DE2" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="DF2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="DG2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="DI2" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="DJ2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="DK2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="DM2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="DN2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="DO2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="DQ2" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="DR2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="DS2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="DU2" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="DV2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="DW2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="DY2" s="6" t="s">
-        <v>181</v>
+      <c r="DX2" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="DZ2" s="2" t="s">
-        <v>258</v>
+        <v>103</v>
       </c>
       <c r="EA2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="EC2" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="ED2" s="2" t="s">
-        <v>258</v>
+        <v>104</v>
+      </c>
+      <c r="EB2" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="EC2" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="EE2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="EG2" s="6" t="s">
-        <v>183</v>
+        <v>103</v>
+      </c>
+      <c r="EF2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="EG2" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="EH2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="EI2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="EL2" s="2" t="s">
-        <v>188</v>
+        <v>107</v>
+      </c>
+      <c r="EJ2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="EK2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="EL2" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="EM2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="EN2" s="7" t="s">
-        <v>187</v>
+        <v>107</v>
       </c>
       <c r="EO2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="EQ2" s="2" t="s">
-        <v>188</v>
+        <v>103</v>
+      </c>
+      <c r="EP2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="EQ2" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="ER2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="ES2" s="7" t="s">
-        <v>187</v>
+        <v>107</v>
       </c>
       <c r="ET2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="EV2" s="2" t="s">
-        <v>188</v>
+        <v>103</v>
+      </c>
+      <c r="EU2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="EV2" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="EW2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="EX2" s="7" t="s">
-        <v>187</v>
+        <v>107</v>
       </c>
       <c r="EY2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="FA2" s="2" t="s">
-        <v>188</v>
+        <v>103</v>
+      </c>
+      <c r="EZ2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="FA2" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="FB2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="FC2" s="7" t="s">
-        <v>187</v>
+        <v>107</v>
       </c>
       <c r="FD2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="FF2" s="2" t="s">
-        <v>188</v>
+        <v>103</v>
+      </c>
+      <c r="FE2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="FF2" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="FG2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="FH2" s="7" t="s">
-        <v>187</v>
+        <v>107</v>
       </c>
       <c r="FI2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="FK2" s="2" t="s">
-        <v>188</v>
+        <v>103</v>
+      </c>
+      <c r="FJ2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="FK2" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="FL2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="FM2" s="7" t="s">
-        <v>187</v>
+        <v>107</v>
       </c>
       <c r="FN2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="FP2" s="2" t="s">
-        <v>188</v>
+        <v>103</v>
+      </c>
+      <c r="FO2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="FP2" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="FQ2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="FR2" s="7" t="s">
-        <v>187</v>
+        <v>107</v>
       </c>
       <c r="FS2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="FU2" s="2" t="s">
-        <v>188</v>
+        <v>103</v>
+      </c>
+      <c r="FT2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="FU2" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="FV2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="FW2" s="7" t="s">
-        <v>187</v>
+        <v>107</v>
       </c>
       <c r="FX2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="FZ2" s="2" t="s">
-        <v>188</v>
+        <v>103</v>
+      </c>
+      <c r="FY2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="FZ2" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="GA2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="GB2" s="7" t="s">
-        <v>187</v>
+        <v>107</v>
       </c>
       <c r="GC2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="GE2" s="2" t="s">
-        <v>188</v>
+        <v>103</v>
+      </c>
+      <c r="GD2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="GE2" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="GF2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="GG2" s="7" t="s">
-        <v>187</v>
+        <v>107</v>
       </c>
       <c r="GH2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="GJ2" s="2" t="s">
-        <v>188</v>
+        <v>103</v>
+      </c>
+      <c r="GI2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="GJ2" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="GK2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="GL2" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="GM2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="GO2" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="GP2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="GQ2" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="GR2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="GT2" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="GU2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="GV2" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="GW2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="GY2" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="GZ2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="HA2" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="HB2" s="2" t="s">
-        <v>192</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>